<commit_message>
dcp-908 test data cleanup
</commit_message>
<xml_diff>
--- a/tests/data/expected/GSE121611.xlsx
+++ b/tests/data/expected/GSE121611.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="4" autoFilterDateGrouping="1" firstSheet="4" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15820" windowWidth="28800" xWindow="0" yWindow="500"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" tabRatio="600" firstSheet="4" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" state="visible" r:id="rId1"/>
@@ -108,36 +108,36 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -542,15 +542,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="2" min="1" style="3" width="25.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="30.6640625"/>
-    <col customWidth="1" max="9" min="4" style="3" width="25.6640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="3" width="28.33203125"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="3" width="22.6640625"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="3" width="23.83203125"/>
+    <col width="25.6640625" customWidth="1" style="3" min="1" max="2"/>
+    <col width="30.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="9"/>
+    <col width="28.33203125" bestFit="1" customWidth="1" style="3" min="10" max="10"/>
+    <col width="22.6640625" bestFit="1" customWidth="1" style="3" min="11" max="11"/>
+    <col width="23.83203125" bestFit="1" customWidth="1" style="3" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>PROJECT LABEL (Required)</t>
@@ -612,7 +612,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="85" r="2" s="3">
+    <row r="2" ht="85" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A short name for the project.</t>
@@ -674,7 +674,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="119" r="3" s="3">
+    <row r="3" ht="119" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Project label is a short label by which you refer to the project. It should have no spaces and should be fewer than 50 characters. For example: CoolOrganProject.</t>
@@ -798,7 +798,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -817,7 +817,11 @@
       <c r="L5" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Single-Cell Transcriptomic Analysis of Human Lung Reveals Complex Multicellular Changes During Pulmonary Fibrosis</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>Pulmonary fibrosis is a heterogeneous syndrome in which fibrotic scar replaces normal lung tissue. We performed massively parallel single-cell RNA-Seq on lung tissue from eight lung transplant donors and eight patients with pulmonary fibrosis. Combined with in situ RNA hybridization, with amplification, these data provide a molecular atlas of disease pathobiology. We identified a distinct, novel population of profibrotic alveolar macrophages exclusively in patients with fibrosis. Within epithelial cells, the expression of genes involved in Wnt secretion and response was restricted to non-overlapping cells. We identified rare cell populations including airway stem cells and senescent cells emerging during pulmonary fibrosis. Analysis of a cryobiopsy specimen from a patient with early disease supports the clinical application of single-cell RNA-Seq to develop personalized approaches to therapy. This dataset contains single-cell RNA-seq data generated from the lungs of the two naive mice, human data for this study has been submitted to dbGap/SRA. Overall design: Single-cell suspension from two 4 mo old C57Bl/6 male mice was prepared and single cell RNA-seq libraries were generated using 3' V2 chemistry kit on Chromium Single cell controller (10x Genomics).</t>
@@ -840,7 +844,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -858,42 +862,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="14" min="1" style="3" width="25.6640625"/>
-    <col hidden="1" max="16" min="15" style="3"/>
-    <col customWidth="1" max="18" min="17" style="3" width="25.6640625"/>
-    <col hidden="1" max="20" min="19" style="3"/>
-    <col customWidth="1" max="23" min="21" style="3" width="25.6640625"/>
-    <col hidden="1" max="25" min="24" style="3"/>
-    <col customWidth="1" max="33" min="26" style="3" width="25.6640625"/>
-    <col customWidth="1" max="34" min="34" style="3" width="26.6640625"/>
-    <col customWidth="1" max="38" min="35" style="3" width="25.6640625"/>
-    <col hidden="1" max="40" min="39" style="3"/>
-    <col customWidth="1" max="42" min="41" style="3" width="25.6640625"/>
-    <col hidden="1" max="44" min="43" style="3"/>
-    <col customWidth="1" max="46" min="45" style="3" width="25.6640625"/>
-    <col customWidth="1" hidden="1" max="48" min="47" style="3" width="8.83203125"/>
-    <col customWidth="1" max="49" min="49" style="3" width="25.6640625"/>
-    <col hidden="1" max="51" min="50" style="3"/>
-    <col customWidth="1" max="52" min="52" style="3" width="25.6640625"/>
-    <col customWidth="1" max="53" min="53" style="3" width="28.6640625"/>
-    <col customWidth="1" max="56" min="54" style="3" width="25.6640625"/>
-    <col customWidth="1" max="57" min="57" style="3" width="27.6640625"/>
-    <col customWidth="1" max="58" min="58" style="3" width="26.6640625"/>
-    <col hidden="1" max="60" min="59" style="3"/>
-    <col customWidth="1" max="61" min="61" style="3" width="25.6640625"/>
-    <col customWidth="1" max="62" min="62" style="3" width="42.6640625"/>
-    <col customWidth="1" max="63" min="63" style="3" width="35.6640625"/>
-    <col customWidth="1" max="64" min="64" style="3" width="33.6640625"/>
-    <col customWidth="1" max="65" min="65" style="3" width="37.6640625"/>
-    <col customWidth="1" max="74" min="66" style="3" width="25.6640625"/>
-    <col hidden="1" max="76" min="75" style="3"/>
-    <col customWidth="1" max="77" min="77" style="3" width="25.6640625"/>
-    <col hidden="1" max="79" min="78" style="3"/>
-    <col customWidth="1" max="80" min="80" style="3" width="25.6640625"/>
-    <col customWidth="1" max="81" min="81" style="3" width="37.6640625"/>
+    <col width="25.6640625" customWidth="1" style="3" min="1" max="14"/>
+    <col hidden="1" style="3" min="15" max="16"/>
+    <col width="25.6640625" customWidth="1" style="3" min="17" max="18"/>
+    <col hidden="1" style="3" min="19" max="20"/>
+    <col width="25.6640625" customWidth="1" style="3" min="21" max="23"/>
+    <col hidden="1" style="3" min="24" max="25"/>
+    <col width="25.6640625" customWidth="1" style="3" min="26" max="33"/>
+    <col width="26.6640625" customWidth="1" style="3" min="34" max="34"/>
+    <col width="25.6640625" customWidth="1" style="3" min="35" max="38"/>
+    <col hidden="1" style="3" min="39" max="40"/>
+    <col width="25.6640625" customWidth="1" style="3" min="41" max="42"/>
+    <col hidden="1" style="3" min="43" max="44"/>
+    <col width="25.6640625" customWidth="1" style="3" min="45" max="46"/>
+    <col hidden="1" width="8.83203125" customWidth="1" style="3" min="47" max="48"/>
+    <col width="25.6640625" customWidth="1" style="3" min="49" max="49"/>
+    <col hidden="1" style="3" min="50" max="51"/>
+    <col width="25.6640625" customWidth="1" style="3" min="52" max="52"/>
+    <col width="28.6640625" customWidth="1" style="3" min="53" max="53"/>
+    <col width="25.6640625" customWidth="1" style="3" min="54" max="56"/>
+    <col width="27.6640625" customWidth="1" style="3" min="57" max="57"/>
+    <col width="26.6640625" customWidth="1" style="3" min="58" max="58"/>
+    <col hidden="1" style="3" min="59" max="60"/>
+    <col width="25.6640625" customWidth="1" style="3" min="61" max="61"/>
+    <col width="42.6640625" customWidth="1" style="3" min="62" max="62"/>
+    <col width="35.6640625" customWidth="1" style="3" min="63" max="63"/>
+    <col width="33.6640625" customWidth="1" style="3" min="64" max="64"/>
+    <col width="37.6640625" customWidth="1" style="3" min="65" max="65"/>
+    <col width="25.6640625" customWidth="1" style="3" min="66" max="74"/>
+    <col hidden="1" style="3" min="75" max="76"/>
+    <col width="25.6640625" customWidth="1" style="3" min="77" max="77"/>
+    <col hidden="1" style="3" min="78" max="79"/>
+    <col width="25.6640625" customWidth="1" style="3" min="80" max="80"/>
+    <col width="37.6640625" customWidth="1" style="3" min="81" max="81"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>CELL LINE ID (Required)</t>
@@ -1300,7 +1304,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the biomaterial.</t>
@@ -1707,7 +1711,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="170" r="3" s="3">
+    <row r="3" ht="170" customHeight="1" s="3">
       <c r="A3" s="2" t="n"/>
       <c r="B3" s="2" t="n"/>
       <c r="C3" s="2" t="n"/>
@@ -2086,7 +2090,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>cell_line.biomaterial_core.biomaterial_id</t>
@@ -2493,7 +2497,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -2581,7 +2585,7 @@
       <c r="CC5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2599,17 +2603,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="3" min="1" style="3" width="25.6640625"/>
-    <col hidden="1" max="5" min="4" style="3"/>
-    <col customWidth="1" max="16" min="6" style="3" width="25.6640625"/>
-    <col hidden="1" max="18" min="17" style="3"/>
-    <col customWidth="1" max="19" min="19" style="3" width="25.6640625"/>
-    <col hidden="1" max="21" min="20" style="3"/>
-    <col customWidth="1" max="22" min="22" style="3" width="25.6640625"/>
-    <col customWidth="1" max="23" min="23" style="3" width="37.6640625"/>
+    <col width="25.6640625" customWidth="1" style="3" min="1" max="3"/>
+    <col hidden="1" style="3" min="4" max="5"/>
+    <col width="25.6640625" customWidth="1" style="3" min="6" max="16"/>
+    <col hidden="1" style="3" min="17" max="18"/>
+    <col width="25.6640625" customWidth="1" style="3" min="19" max="19"/>
+    <col hidden="1" style="3" min="20" max="21"/>
+    <col width="25.6640625" customWidth="1" style="3" min="22" max="22"/>
+    <col width="37.6640625" customWidth="1" style="3" min="23" max="23"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>FILE NAME (Required)</t>
@@ -2726,7 +2730,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>The name of the file.</t>
@@ -2843,7 +2847,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="153" r="3" s="3">
+    <row r="3" ht="153" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Include the file extension in the file name. For example: R1.fastq.gz; codebook.json</t>
@@ -2948,7 +2952,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>supplementary_file.file_core.file_name</t>
@@ -3065,7 +3069,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -3095,7 +3099,7 @@
       <c r="W5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3113,21 +3117,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="3" min="1" style="3" width="25.6640625"/>
-    <col hidden="1" max="5" min="4" style="3"/>
-    <col customWidth="1" max="11" min="6" style="3" width="25.6640625"/>
-    <col customWidth="1" max="12" min="12" style="3" width="35.6640625"/>
-    <col customWidth="1" max="13" min="13" style="3" width="42.6640625"/>
-    <col customWidth="1" max="14" min="14" style="3" width="33.6640625"/>
-    <col customWidth="1" max="23" min="15" style="3" width="25.6640625"/>
-    <col hidden="1" max="25" min="24" style="3"/>
-    <col customWidth="1" max="26" min="26" style="3" width="25.6640625"/>
-    <col hidden="1" max="28" min="27" style="3"/>
-    <col customWidth="1" max="29" min="29" style="3" width="25.6640625"/>
-    <col customWidth="1" max="30" min="30" style="3" width="37.6640625"/>
+    <col width="25.6640625" customWidth="1" style="3" min="1" max="3"/>
+    <col hidden="1" style="3" min="4" max="5"/>
+    <col width="25.6640625" customWidth="1" style="3" min="6" max="11"/>
+    <col width="35.6640625" customWidth="1" style="3" min="12" max="12"/>
+    <col width="42.6640625" customWidth="1" style="3" min="13" max="13"/>
+    <col width="33.6640625" customWidth="1" style="3" min="14" max="14"/>
+    <col width="25.6640625" customWidth="1" style="3" min="15" max="23"/>
+    <col hidden="1" style="3" min="24" max="25"/>
+    <col width="25.6640625" customWidth="1" style="3" min="26" max="26"/>
+    <col hidden="1" style="3" min="27" max="28"/>
+    <col width="25.6640625" customWidth="1" style="3" min="29" max="29"/>
+    <col width="37.6640625" customWidth="1" style="3" min="30" max="30"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>FILE NAME (Required)</t>
@@ -3279,7 +3283,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>The name of the file.</t>
@@ -3431,7 +3435,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="153" r="3" s="3">
+    <row r="3" ht="153" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Include the file extension in the file name. For example: R1.fastq.gz; codebook.json</t>
@@ -3567,7 +3571,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>sequence_file.file_core.file_name</t>
@@ -3719,7 +3723,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -4180,7 +4184,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4198,20 +4202,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="3" min="1" style="3" width="25.6640625"/>
-    <col hidden="1" max="5" min="4" style="3"/>
-    <col customWidth="1" max="6" min="6" style="3" width="25.6640625"/>
-    <col customWidth="1" max="7" min="7" style="3" width="35.6640625"/>
-    <col customWidth="1" max="8" min="8" style="3" width="30.6640625"/>
-    <col customWidth="1" max="17" min="9" style="3" width="25.6640625"/>
-    <col hidden="1" max="19" min="18" style="3"/>
-    <col customWidth="1" max="20" min="20" style="3" width="25.6640625"/>
-    <col hidden="1" max="22" min="21" style="3"/>
-    <col customWidth="1" max="23" min="23" style="3" width="25.6640625"/>
-    <col customWidth="1" max="24" min="24" style="3" width="37.6640625"/>
+    <col width="25.6640625" customWidth="1" style="3" min="1" max="3"/>
+    <col hidden="1" style="3" min="4" max="5"/>
+    <col width="25.6640625" customWidth="1" style="3" min="6" max="6"/>
+    <col width="35.6640625" customWidth="1" style="3" min="7" max="7"/>
+    <col width="30.6640625" customWidth="1" style="3" min="8" max="8"/>
+    <col width="25.6640625" customWidth="1" style="3" min="9" max="17"/>
+    <col hidden="1" style="3" min="18" max="19"/>
+    <col width="25.6640625" customWidth="1" style="3" min="20" max="20"/>
+    <col hidden="1" style="3" min="21" max="22"/>
+    <col width="25.6640625" customWidth="1" style="3" min="23" max="23"/>
+    <col width="37.6640625" customWidth="1" style="3" min="24" max="24"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>FILE NAME (Required)</t>
@@ -4333,7 +4337,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>The name of the file.</t>
@@ -4455,7 +4459,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="153" r="3" s="3">
+    <row r="3" ht="153" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Include the file extension in the file name. For example: R1.fastq.gz; codebook.json</t>
@@ -4561,7 +4565,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>image_file.file_core.file_name</t>
@@ -4683,7 +4687,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -4714,7 +4718,7 @@
       <c r="X5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4732,16 +4736,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="33.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="25.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="31.6640625"/>
-    <col customWidth="1" max="6" min="4" style="3" width="25.6640625"/>
-    <col customWidth="1" max="7" min="7" style="3" width="28.6640625"/>
-    <col hidden="1" max="9" min="8" style="3"/>
-    <col customWidth="1" max="15" min="10" style="3" width="25.6640625"/>
+    <col width="33.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="25.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="31.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="6"/>
+    <col width="28.6640625" customWidth="1" style="3" min="7" max="7"/>
+    <col hidden="1" style="3" min="8" max="9"/>
+    <col width="25.6640625" customWidth="1" style="3" min="10" max="15"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>COLLECTION PROTOCOL ID (Required)</t>
@@ -4818,7 +4822,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the protocol.</t>
@@ -4895,7 +4899,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="136" r="3" s="3">
+    <row r="3" ht="136" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Protocol ID should have no spaces.</t>
@@ -4964,7 +4968,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>collection_protocol.protocol_core.protocol_id</t>
@@ -5041,7 +5045,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -5063,7 +5067,7 @@
       <c r="O5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5081,16 +5085,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="35.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="26.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="33.6640625"/>
-    <col customWidth="1" max="6" min="4" style="3" width="25.6640625"/>
-    <col customWidth="1" max="7" min="7" style="3" width="30.6640625"/>
-    <col hidden="1" max="9" min="8" style="3"/>
-    <col customWidth="1" max="15" min="10" style="3" width="25.6640625"/>
+    <col width="35.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="26.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="33.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="6"/>
+    <col width="30.6640625" customWidth="1" style="3" min="7" max="7"/>
+    <col hidden="1" style="3" min="8" max="9"/>
+    <col width="25.6640625" customWidth="1" style="3" min="10" max="15"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>DISSOCIATION PROTOCOL ID (Required)</t>
@@ -5167,7 +5171,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the protocol.</t>
@@ -5244,7 +5248,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="136" r="3" s="3">
+    <row r="3" ht="136" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Protocol ID should have no spaces.</t>
@@ -5313,7 +5317,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>dissociation_protocol.protocol_core.protocol_id</t>
@@ -5390,7 +5394,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -5412,7 +5416,7 @@
       <c r="O5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5430,17 +5434,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="38.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="29.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="36.6640625"/>
-    <col customWidth="1" max="6" min="4" style="3" width="25.6640625"/>
-    <col customWidth="1" max="7" min="7" style="3" width="33.6640625"/>
-    <col customWidth="1" max="17" min="8" style="3" width="25.6640625"/>
-    <col customWidth="1" max="18" min="18" style="3" width="33.6640625"/>
-    <col customWidth="1" max="19" min="19" style="3" width="25.6640625"/>
+    <col width="38.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="29.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="36.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="6"/>
+    <col width="33.6640625" customWidth="1" style="3" min="7" max="7"/>
+    <col width="25.6640625" customWidth="1" style="3" min="8" max="17"/>
+    <col width="33.6640625" customWidth="1" style="3" min="18" max="18"/>
+    <col width="25.6640625" customWidth="1" style="3" min="19" max="19"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>DIFFERENTIATION PROTOCOL ID (Required)</t>
@@ -5537,7 +5541,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="68" r="2" s="3">
+    <row r="2" ht="68" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the protocol.</t>
@@ -5634,7 +5638,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="85" r="3" s="3">
+    <row r="3" ht="85" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Protocol ID should have no spaces.</t>
@@ -5723,7 +5727,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>differentiation_protocol.protocol_core.protocol_id</t>
@@ -5820,7 +5824,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -5846,7 +5850,7 @@
       <c r="S5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5864,16 +5868,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="33.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="25.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="31.6640625"/>
-    <col customWidth="1" max="6" min="4" style="3" width="25.6640625"/>
-    <col customWidth="1" max="7" min="7" style="3" width="28.6640625"/>
-    <col hidden="1" max="9" min="8" style="3"/>
-    <col customWidth="1" max="12" min="10" style="3" width="25.6640625"/>
+    <col width="33.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="25.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="31.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="6"/>
+    <col width="28.6640625" customWidth="1" style="3" min="7" max="7"/>
+    <col hidden="1" style="3" min="8" max="9"/>
+    <col width="25.6640625" customWidth="1" style="3" min="10" max="12"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>ENRICHMENT PROTOCOL ID (Required)</t>
@@ -5935,7 +5939,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the protocol.</t>
@@ -5997,7 +6001,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="136" r="3" s="3">
+    <row r="3" ht="136" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Protocol ID should have no spaces.</t>
@@ -6051,7 +6055,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>enrichment_protocol.protocol_core.protocol_id</t>
@@ -6113,7 +6117,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -6132,7 +6136,7 @@
       <c r="L5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -6150,15 +6154,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="43.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="34.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="41.6640625"/>
-    <col customWidth="1" max="6" min="4" style="3" width="25.6640625"/>
-    <col customWidth="1" max="7" min="7" style="3" width="37.6640625"/>
-    <col customWidth="1" max="8" min="8" style="3" width="25.6640625"/>
+    <col width="43.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="34.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="41.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="6"/>
+    <col width="37.6640625" customWidth="1" style="3" min="7" max="7"/>
+    <col width="25.6640625" customWidth="1" style="3" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>AGGREGATE GENERATION PROTOCOL ID (Required)</t>
@@ -6200,7 +6204,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="51" r="2" s="3">
+    <row r="2" ht="51" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the protocol.</t>
@@ -6242,7 +6246,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="85" r="3" s="3">
+    <row r="3" ht="85" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Protocol ID should have no spaces.</t>
@@ -6276,7 +6280,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>aggregate_generation_protocol.protocol_core.protocol_id</t>
@@ -6318,7 +6322,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -6333,7 +6337,7 @@
       <c r="H5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -6351,22 +6355,22 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="37.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="28.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="35.6640625"/>
-    <col customWidth="1" max="6" min="4" style="3" width="25.6640625"/>
-    <col customWidth="1" max="7" min="7" style="3" width="27.6640625"/>
-    <col customWidth="1" max="8" min="8" style="3" width="25.6640625"/>
-    <col customWidth="1" max="9" min="9" style="3" width="27.6640625"/>
-    <col customWidth="1" max="10" min="10" style="3" width="30.6640625"/>
-    <col customWidth="1" max="11" min="11" style="3" width="28.6640625"/>
-    <col customWidth="1" max="12" min="12" style="3" width="32.6640625"/>
-    <col customWidth="1" max="13" min="13" style="3" width="27.6640625"/>
-    <col customWidth="1" max="16" min="14" style="3" width="25.6640625"/>
-    <col customWidth="1" max="17" min="17" style="3" width="26.6640625"/>
+    <col width="37.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="28.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="35.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="6"/>
+    <col width="27.6640625" customWidth="1" style="3" min="7" max="7"/>
+    <col width="25.6640625" customWidth="1" style="3" min="8" max="8"/>
+    <col width="27.6640625" customWidth="1" style="3" min="9" max="9"/>
+    <col width="30.6640625" customWidth="1" style="3" min="10" max="10"/>
+    <col width="28.6640625" customWidth="1" style="3" min="11" max="11"/>
+    <col width="32.6640625" customWidth="1" style="3" min="12" max="12"/>
+    <col width="27.6640625" customWidth="1" style="3" min="13" max="13"/>
+    <col width="25.6640625" customWidth="1" style="3" min="14" max="16"/>
+    <col width="26.6640625" customWidth="1" style="3" min="17" max="17"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>IPSC INDUCTION PROTOCOL ID (Required)</t>
@@ -6453,7 +6457,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="68" r="2" s="3">
+    <row r="2" ht="68" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the protocol.</t>
@@ -6540,7 +6544,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="85" r="3" s="3">
+    <row r="3" ht="85" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Protocol ID should have no spaces.</t>
@@ -6619,7 +6623,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>ipsc_induction_protocol.protocol_core.protocol_id</t>
@@ -6706,7 +6710,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -6730,7 +6734,7 @@
       <c r="Q5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -6740,7 +6744,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6748,12 +6752,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="9" min="1" style="3" width="25.6640625"/>
-    <col hidden="1" max="11" min="10" style="3"/>
-    <col customWidth="1" max="12" min="12" style="3" width="25.6640625"/>
+    <col width="25.6640625" customWidth="1" style="3" min="1" max="9"/>
+    <col hidden="1" style="3" min="10" max="11"/>
+    <col width="25.6640625" customWidth="1" style="3" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>CONTACT NAME (Required)</t>
@@ -6815,7 +6819,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Name of individual who has contributed to the project.</t>
@@ -6877,7 +6881,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="136" r="3" s="3">
+    <row r="3" ht="136" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Enter in the format: first name,middle name or initial,last name. For example: John,D,Doe; Jane,,Smith</t>
@@ -6939,7 +6943,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>project.contributors.name</t>
@@ -7001,7 +7005,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -7019,9 +7023,596 @@
       <c r="K5" s="1" t="n"/>
       <c r="L5" s="1" t="n"/>
     </row>
-    <row r="6"/>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Paul A,,Reyfman</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>James M,,Walter</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Nikita,,Joshi</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kishore R,,Anekalla</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Alexandra C,,McQuattie-Pimentel</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Stephen,,Chiu</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2 Division of Thoracic Surgery, Department of Surgery.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Ramiro,,Fernandez</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2 Division of Thoracic Surgery, Department of Surgery.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mahzad,,Akbarpour</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2 Division of Thoracic Surgery, Department of Surgery.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ching-I,,Chen</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Ziyou,,Ren</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Rohan,,Verma</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Hiam,,Abdala-Valencia</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Kiwon,,Nam</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Monica,,Chi</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>SeungHye,,Han</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Francisco J,,Gonzalez-Gonzalez</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Saul,,Soberanes</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Satoshi,,Watanabe</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Kinola J N,,Williams</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Annette S,,Flozak</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Trevor T,,Nicholson</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Vince K,,Morgan</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>3 Division of Rheumatology, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Deborah R,,Winter</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>3 Division of Rheumatology, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Monique,,Hinchcliff</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>3 Division of Rheumatology, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Cara L,,Hrusch</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>4 Section of Pulmonary and Critical Care Medicine, University of Chicago, Chicago, Illinois; and.</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Robert D,,Guzy</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>4 Section of Pulmonary and Critical Care Medicine, University of Chicago, Chicago, Illinois; and.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Catherine A,,Bonham</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>4 Section of Pulmonary and Critical Care Medicine, University of Chicago, Chicago, Illinois; and.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Anne I,,Sperling</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>4 Section of Pulmonary and Critical Care Medicine, University of Chicago, Chicago, Illinois; and.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Remzi,,Bag</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>4 Section of Pulmonary and Critical Care Medicine, University of Chicago, Chicago, Illinois; and.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Robert B,,Hamanaka</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>4 Section of Pulmonary and Critical Care Medicine, University of Chicago, Chicago, Illinois; and.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Gökhan M,,Mutlu</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>4 Section of Pulmonary and Critical Care Medicine, University of Chicago, Chicago, Illinois; and.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Anjana V,,Yeldandi</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>5 Department of Pathology, and.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Stacy A,,Marshall</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>6 Department of Biochemistry and Molecular Genetics, Feinberg School of Medicine, Northwestern University, Chicago, Illinois.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Ali,,Shilatifard</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>6 Department of Biochemistry and Molecular Genetics, Feinberg School of Medicine, Northwestern University, Chicago, Illinois.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Luis A N,,Amaral</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>7 Department of Chemical and Biological Engineering, Weinberg College of Arts and Sciences, Northwestern University, Evanston, Illinois.</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Harris,,Perlman</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>3 Division of Rheumatology, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Jacob I,,Sznajder</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>A Christine,,Argento</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Colin T,,Gillespie</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Jane,,Dematte</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Manu,,Jain</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Benjamin D,,Singer</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Karen M,,Ridge</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Anna P,,Lam</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Ankit,,Bharat</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2 Division of Thoracic Surgery, Department of Surgery.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Sangeeta M,,Bhorade</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Cara J,,Gottardi</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>G R Scott,,Budinger</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Alexander V,,Misharin</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>1 Division of Pulmonary and Critical Care Medicine, Department of Medicine.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -7039,23 +7630,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="42.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="33.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="40.6640625"/>
-    <col customWidth="1" max="9" min="4" style="3" width="25.6640625"/>
-    <col customWidth="1" max="10" min="10" style="3" width="40.6640625"/>
-    <col customWidth="1" max="11" min="11" style="3" width="33.6640625"/>
-    <col hidden="1" max="13" min="12" style="3"/>
-    <col customWidth="1" max="16" min="14" style="3" width="25.6640625"/>
-    <col hidden="1" max="18" min="17" style="3"/>
-    <col customWidth="1" max="19" min="19" style="3" width="25.6640625"/>
-    <col customWidth="1" max="20" min="20" style="3" width="27.6640625"/>
-    <col customWidth="1" max="21" min="21" style="3" width="37.6640625"/>
-    <col hidden="1" max="23" min="22" style="3"/>
-    <col customWidth="1" max="25" min="24" style="3" width="25.6640625"/>
+    <col width="42.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="33.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="40.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="9"/>
+    <col width="40.6640625" customWidth="1" style="3" min="10" max="10"/>
+    <col width="33.6640625" customWidth="1" style="3" min="11" max="11"/>
+    <col hidden="1" style="3" min="12" max="13"/>
+    <col width="25.6640625" customWidth="1" style="3" min="14" max="16"/>
+    <col hidden="1" style="3" min="17" max="18"/>
+    <col width="25.6640625" customWidth="1" style="3" min="19" max="19"/>
+    <col width="27.6640625" customWidth="1" style="3" min="20" max="20"/>
+    <col width="37.6640625" customWidth="1" style="3" min="21" max="21"/>
+    <col hidden="1" style="3" min="22" max="23"/>
+    <col width="25.6640625" customWidth="1" style="3" min="24" max="25"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>IMAGING PREPARATION PROTOCOL ID (Required)</t>
@@ -7182,7 +7773,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the protocol.</t>
@@ -7309,7 +7900,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="102" r="3" s="3">
+    <row r="3" ht="102" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Protocol ID should have no spaces.</t>
@@ -7428,7 +8019,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>imaging_preparation_protocol.protocol_core.protocol_id</t>
@@ -7555,7 +8146,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -7587,7 +8178,7 @@
       <c r="Y5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -7605,22 +8196,22 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="30.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="25.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="28.6640625"/>
-    <col customWidth="1" max="6" min="4" style="3" width="25.6640625"/>
-    <col customWidth="1" max="7" min="7" style="3" width="28.6640625"/>
-    <col customWidth="1" max="8" min="8" style="3" width="31.6640625"/>
-    <col hidden="1" max="10" min="9" style="3"/>
-    <col customWidth="1" max="11" min="11" style="3" width="25.6640625"/>
-    <col customWidth="1" max="12" min="12" style="3" width="29.6640625"/>
-    <col customWidth="1" max="13" min="13" style="3" width="25.6640625"/>
-    <col customWidth="1" max="14" min="14" style="3" width="40.6640625"/>
-    <col customWidth="1" max="20" min="15" style="3" width="25.6640625"/>
-    <col customWidth="1" max="21" min="21" style="3" width="28.6640625"/>
+    <col width="30.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="25.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="28.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="6"/>
+    <col width="28.6640625" customWidth="1" style="3" min="7" max="7"/>
+    <col width="31.6640625" customWidth="1" style="3" min="8" max="8"/>
+    <col hidden="1" style="3" min="9" max="10"/>
+    <col width="25.6640625" customWidth="1" style="3" min="11" max="11"/>
+    <col width="29.6640625" customWidth="1" style="3" min="12" max="12"/>
+    <col width="25.6640625" customWidth="1" style="3" min="13" max="13"/>
+    <col width="40.6640625" customWidth="1" style="3" min="14" max="14"/>
+    <col width="25.6640625" customWidth="1" style="3" min="15" max="20"/>
+    <col width="28.6640625" customWidth="1" style="3" min="21" max="21"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>IMAGING PROTOCOL ID (Required)</t>
@@ -7727,7 +8318,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the protocol.</t>
@@ -7834,7 +8425,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="153" r="3" s="3">
+    <row r="3" ht="153" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Protocol ID should have no spaces.</t>
@@ -7933,7 +8524,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>imaging_protocol.protocol_core.protocol_id</t>
@@ -8040,7 +8631,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -8068,7 +8659,7 @@
       <c r="U5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -8086,50 +8677,50 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="42.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="33.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="40.6640625"/>
-    <col customWidth="1" max="6" min="4" style="3" width="25.6640625"/>
-    <col customWidth="1" max="7" min="7" style="3" width="49.6640625"/>
-    <col customWidth="1" max="9" min="8" style="3" width="40.6640625"/>
-    <col customWidth="1" max="10" min="10" style="3" width="38.6640625"/>
-    <col customWidth="1" max="14" min="11" style="3" width="25.6640625"/>
-    <col customWidth="1" max="15" min="15" style="3" width="38.6640625"/>
-    <col hidden="1" max="17" min="16" style="3"/>
-    <col customWidth="1" max="18" min="18" style="3" width="30.6640625"/>
-    <col customWidth="1" max="19" min="19" style="3" width="38.6640625"/>
-    <col hidden="1" max="21" min="20" style="3"/>
-    <col customWidth="1" max="22" min="22" style="3" width="38.6640625"/>
-    <col customWidth="1" max="23" min="23" style="3" width="41.6640625"/>
-    <col customWidth="1" max="24" min="24" style="3" width="39.6640625"/>
-    <col customWidth="1" max="25" min="25" style="3" width="43.6640625"/>
-    <col customWidth="1" max="26" min="26" style="3" width="38.6640625"/>
-    <col customWidth="1" max="27" min="27" style="3" width="32.6640625"/>
-    <col customWidth="1" max="28" min="28" style="3" width="41.6640625"/>
-    <col customWidth="1" max="29" min="29" style="3" width="44.6640625"/>
-    <col customWidth="1" max="30" min="30" style="3" width="42.6640625"/>
-    <col customWidth="1" max="31" min="31" style="3" width="46.6640625"/>
-    <col customWidth="1" max="32" min="32" style="3" width="41.6640625"/>
-    <col customWidth="1" max="33" min="33" style="3" width="35.6640625"/>
-    <col customWidth="1" max="36" min="34" style="3" width="25.6640625"/>
-    <col customWidth="1" max="37" min="37" style="3" width="26.6640625"/>
-    <col customWidth="1" max="38" min="38" style="3" width="29.6640625"/>
-    <col customWidth="1" max="39" min="39" style="3" width="27.6640625"/>
-    <col customWidth="1" max="40" min="40" style="3" width="31.6640625"/>
-    <col customWidth="1" max="41" min="41" style="3" width="26.6640625"/>
-    <col customWidth="1" max="43" min="42" style="3" width="25.6640625"/>
-    <col customWidth="1" max="44" min="44" style="3" width="48.6640625"/>
-    <col customWidth="1" max="46" min="45" style="3" width="39.6640625"/>
-    <col customWidth="1" max="47" min="47" style="3" width="37.6640625"/>
-    <col customWidth="1" max="48" min="48" style="3" width="32.6640625"/>
-    <col hidden="1" max="50" min="49" style="3"/>
-    <col customWidth="1" max="51" min="51" style="3" width="33.6640625"/>
-    <col hidden="1" max="53" min="52" style="3"/>
-    <col customWidth="1" max="54" min="54" style="3" width="25.6640625"/>
-    <col customWidth="1" max="55" min="55" style="3" width="26.6640625"/>
+    <col width="42.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="33.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="40.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="6"/>
+    <col width="49.6640625" customWidth="1" style="3" min="7" max="7"/>
+    <col width="40.6640625" customWidth="1" style="3" min="8" max="9"/>
+    <col width="38.6640625" customWidth="1" style="3" min="10" max="10"/>
+    <col width="25.6640625" customWidth="1" style="3" min="11" max="14"/>
+    <col width="38.6640625" customWidth="1" style="3" min="15" max="15"/>
+    <col hidden="1" style="3" min="16" max="17"/>
+    <col width="30.6640625" customWidth="1" style="3" min="18" max="18"/>
+    <col width="38.6640625" customWidth="1" style="3" min="19" max="19"/>
+    <col hidden="1" style="3" min="20" max="21"/>
+    <col width="38.6640625" customWidth="1" style="3" min="22" max="22"/>
+    <col width="41.6640625" customWidth="1" style="3" min="23" max="23"/>
+    <col width="39.6640625" customWidth="1" style="3" min="24" max="24"/>
+    <col width="43.6640625" customWidth="1" style="3" min="25" max="25"/>
+    <col width="38.6640625" customWidth="1" style="3" min="26" max="26"/>
+    <col width="32.6640625" customWidth="1" style="3" min="27" max="27"/>
+    <col width="41.6640625" customWidth="1" style="3" min="28" max="28"/>
+    <col width="44.6640625" customWidth="1" style="3" min="29" max="29"/>
+    <col width="42.6640625" customWidth="1" style="3" min="30" max="30"/>
+    <col width="46.6640625" customWidth="1" style="3" min="31" max="31"/>
+    <col width="41.6640625" customWidth="1" style="3" min="32" max="32"/>
+    <col width="35.6640625" customWidth="1" style="3" min="33" max="33"/>
+    <col width="25.6640625" customWidth="1" style="3" min="34" max="36"/>
+    <col width="26.6640625" customWidth="1" style="3" min="37" max="37"/>
+    <col width="29.6640625" customWidth="1" style="3" min="38" max="38"/>
+    <col width="27.6640625" customWidth="1" style="3" min="39" max="39"/>
+    <col width="31.6640625" customWidth="1" style="3" min="40" max="40"/>
+    <col width="26.6640625" customWidth="1" style="3" min="41" max="41"/>
+    <col width="25.6640625" customWidth="1" style="3" min="42" max="43"/>
+    <col width="48.6640625" customWidth="1" style="3" min="44" max="44"/>
+    <col width="39.6640625" customWidth="1" style="3" min="45" max="46"/>
+    <col width="37.6640625" customWidth="1" style="3" min="47" max="47"/>
+    <col width="32.6640625" customWidth="1" style="3" min="48" max="48"/>
+    <col hidden="1" style="3" min="49" max="50"/>
+    <col width="33.6640625" customWidth="1" style="3" min="51" max="51"/>
+    <col hidden="1" style="3" min="52" max="53"/>
+    <col width="25.6640625" customWidth="1" style="3" min="54" max="54"/>
+    <col width="26.6640625" customWidth="1" style="3" min="55" max="55"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="43" r="1" s="6">
+    <row r="1" ht="43" customFormat="1" customHeight="1" s="6">
       <c r="A1" s="5" t="inlineStr">
         <is>
           <t>LIBRARY PREPARATION PROTOCOL ID (Required)</t>
@@ -8406,7 +8997,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="142" r="2" s="3">
+    <row r="2" ht="142" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the protocol.</t>
@@ -8683,7 +9274,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="142" r="3" s="3">
+    <row r="3" ht="142" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Protocol ID should have no spaces.</t>
@@ -8952,7 +9543,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>library_preparation_protocol.protocol_core.protocol_id</t>
@@ -9229,7 +9820,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -9290,66 +9881,9 @@
       <c r="BB5" s="1" t="n"/>
       <c r="BC5" s="1" t="n"/>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>library_protocol_1</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Read1</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>12</v>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>polyA RNA</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>single cell</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>Drop-seq</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="AH6" t="inlineStr"/>
-      <c r="AI6" t="inlineStr">
-        <is>
-          <t>poly-dT</t>
-        </is>
-      </c>
-      <c r="AJ6" t="inlineStr">
-        <is>
-          <t>first</t>
-        </is>
-      </c>
-      <c r="AR6" t="inlineStr">
-        <is>
-          <t>Read1</t>
-        </is>
-      </c>
-      <c r="AS6" t="n">
-        <v>12</v>
-      </c>
-      <c r="AT6" t="n">
-        <v>8</v>
-      </c>
-    </row>
+    <row r="6"/>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -9367,21 +9901,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="33.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="25.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="31.6640625"/>
-    <col customWidth="1" max="6" min="4" style="3" width="25.6640625"/>
-    <col customWidth="1" max="7" min="7" style="3" width="44.6640625"/>
-    <col hidden="1" max="9" min="8" style="3"/>
-    <col customWidth="1" max="11" min="10" style="3" width="25.6640625"/>
-    <col customWidth="1" max="12" min="12" style="3" width="28.6640625"/>
-    <col hidden="1" max="14" min="13" style="3"/>
-    <col customWidth="1" max="15" min="15" style="3" width="25.6640625"/>
-    <col customWidth="1" max="16" min="16" style="3" width="29.6640625"/>
-    <col customWidth="1" max="18" min="17" style="3" width="25.6640625"/>
+    <col width="33.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="25.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="31.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="6"/>
+    <col width="44.6640625" customWidth="1" style="3" min="7" max="7"/>
+    <col hidden="1" style="3" min="8" max="9"/>
+    <col width="25.6640625" customWidth="1" style="3" min="10" max="11"/>
+    <col width="28.6640625" customWidth="1" style="3" min="12" max="12"/>
+    <col hidden="1" style="3" min="13" max="14"/>
+    <col width="25.6640625" customWidth="1" style="3" min="15" max="15"/>
+    <col width="29.6640625" customWidth="1" style="3" min="16" max="16"/>
+    <col width="25.6640625" customWidth="1" style="3" min="17" max="18"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>SEQUENCING PROTOCOL ID (Required)</t>
@@ -9473,7 +10007,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the protocol.</t>
@@ -9565,7 +10099,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="221" r="3" s="3">
+    <row r="3" ht="221" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Protocol ID should have no spaces.</t>
@@ -9649,7 +10183,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>sequencing_protocol.protocol_core.protocol_id</t>
@@ -9741,7 +10275,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -9776,7 +10310,7 @@
       <c r="L6" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -9794,31 +10328,31 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="3" width="38.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="38.6640625"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="3" width="42.6640625"/>
-    <col customWidth="1" max="5" min="4" style="3" width="58.83203125"/>
-    <col customWidth="1" max="6" min="6" style="3" width="24.6640625"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="3" width="25"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="3" width="39"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="3" width="38.83203125"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="3" width="55"/>
-    <col customWidth="1" max="11" min="11" style="3" width="18.6640625"/>
-    <col customWidth="1" max="12" min="12" style="3" width="23.6640625"/>
-    <col customWidth="1" max="17" min="13" style="3" width="18.6640625"/>
-    <col customWidth="1" max="18" min="18" style="3" width="23.6640625"/>
-    <col customWidth="1" max="20" min="19" style="3" width="8.83203125"/>
-    <col customWidth="1" max="21" min="21" style="3" width="18.6640625"/>
-    <col bestFit="1" customWidth="1" max="22" min="22" style="3" width="31.33203125"/>
-    <col bestFit="1" customWidth="1" max="23" min="23" style="3" width="25.1640625"/>
-    <col customWidth="1" max="24" min="24" style="3" width="27.6640625"/>
-    <col customWidth="1" max="25" min="25" style="3" width="30.6640625"/>
-    <col bestFit="1" customWidth="1" max="26" min="26" style="3" width="43.83203125"/>
-    <col customWidth="1" max="28" min="27" style="3" width="8.83203125"/>
-    <col customWidth="1" max="16384" min="29" style="3" width="8.83203125"/>
+    <col width="38.6640625" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="38.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="42.6640625" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
+    <col width="58.83203125" customWidth="1" style="3" min="4" max="5"/>
+    <col width="24.6640625" customWidth="1" style="3" min="6" max="6"/>
+    <col width="25" bestFit="1" customWidth="1" style="3" min="7" max="7"/>
+    <col width="39" bestFit="1" customWidth="1" style="3" min="8" max="8"/>
+    <col width="38.83203125" bestFit="1" customWidth="1" style="3" min="9" max="9"/>
+    <col width="55" bestFit="1" customWidth="1" style="3" min="10" max="10"/>
+    <col width="18.6640625" customWidth="1" style="3" min="11" max="11"/>
+    <col width="23.6640625" customWidth="1" style="3" min="12" max="12"/>
+    <col width="18.6640625" customWidth="1" style="3" min="13" max="17"/>
+    <col width="23.6640625" customWidth="1" style="3" min="18" max="18"/>
+    <col width="8.83203125" customWidth="1" style="3" min="19" max="20"/>
+    <col width="18.6640625" customWidth="1" style="3" min="21" max="21"/>
+    <col width="31.33203125" bestFit="1" customWidth="1" style="3" min="22" max="22"/>
+    <col width="25.1640625" bestFit="1" customWidth="1" style="3" min="23" max="23"/>
+    <col width="27.6640625" customWidth="1" style="3" min="24" max="24"/>
+    <col width="30.6640625" customWidth="1" style="3" min="25" max="25"/>
+    <col width="43.83203125" bestFit="1" customWidth="1" style="3" min="26" max="26"/>
+    <col width="8.83203125" customWidth="1" style="3" min="27" max="28"/>
+    <col width="8.83203125" customWidth="1" style="3" min="29" max="16384"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="50" r="1" s="3">
+    <row r="1" ht="50" customHeight="1" s="3">
       <c r="A1" s="5" t="inlineStr">
         <is>
           <t>FILE NAME (Required)</t>
@@ -9960,7 +10494,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="50" r="2" s="3">
+    <row r="2" ht="50" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>The name of the file.</t>
@@ -10102,7 +10636,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="108" r="3" s="3">
+    <row r="3" ht="108" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Include the file extension in the file name. For example: R1.fastq.gz; codebook.json</t>
@@ -10212,7 +10746,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="27" r="4" s="3">
+    <row r="4" ht="27" customHeight="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>analysis_file.file_core.file_name</t>
@@ -10354,7 +10888,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="5" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -10781,7 +11315,7 @@
       <c r="R103" s="8" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -10793,29 +11327,29 @@
   </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0" zoomScale="81" zoomScaleNormal="81">
+    <sheetView topLeftCell="C1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="28.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="30.6640625"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="3" width="84.6640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="3" width="39.33203125"/>
-    <col customWidth="1" max="5" min="5" style="3" width="18.6640625"/>
-    <col bestFit="1" customWidth="1" max="7" min="6" style="3" width="33.1640625"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="3" width="31.33203125"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="3" width="34.33203125"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="3" width="58.83203125"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="3" width="32.1640625"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="3" width="38.6640625"/>
-    <col customWidth="1" max="14" min="13" style="3" width="18.6640625"/>
-    <col customWidth="1" max="17" min="15" style="3" width="8.83203125"/>
-    <col customWidth="1" max="16384" min="18" style="3" width="8.83203125"/>
+    <col width="28.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="30.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="84.6640625" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
+    <col width="39.33203125" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
+    <col width="18.6640625" customWidth="1" style="3" min="5" max="5"/>
+    <col width="33.1640625" bestFit="1" customWidth="1" style="3" min="6" max="7"/>
+    <col width="31.33203125" bestFit="1" customWidth="1" style="3" min="8" max="8"/>
+    <col width="34.33203125" bestFit="1" customWidth="1" style="3" min="9" max="9"/>
+    <col width="58.83203125" bestFit="1" customWidth="1" style="3" min="10" max="10"/>
+    <col width="32.1640625" bestFit="1" customWidth="1" style="3" min="11" max="11"/>
+    <col width="38.6640625" bestFit="1" customWidth="1" style="3" min="12" max="12"/>
+    <col width="18.6640625" customWidth="1" style="3" min="13" max="14"/>
+    <col width="8.83203125" customWidth="1" style="3" min="15" max="17"/>
+    <col width="8.83203125" customWidth="1" style="3" min="18" max="16384"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="50" r="1" s="3">
+    <row r="1" ht="50" customHeight="1" s="3">
       <c r="A1" s="5" t="inlineStr">
         <is>
           <t>ANALYSIS PROTOCOL ID</t>
@@ -10876,7 +11410,7 @@
       <c r="N1" s="5" t="n"/>
       <c r="O1" s="5" t="n"/>
     </row>
-    <row customHeight="1" ht="50" r="2" s="3">
+    <row r="2" ht="50" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the protocol.</t>
@@ -10921,7 +11455,7 @@
       <c r="N2" s="2" t="n"/>
       <c r="O2" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="119" r="3" s="3">
+    <row r="3" ht="119" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Protocol ID should have no spaces.</t>
@@ -10958,7 +11492,7 @@
       <c r="N3" s="2" t="n"/>
       <c r="O3" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="34" r="4" s="3">
+    <row r="4" ht="34" customHeight="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>analysis_protocol.protocol_core.protocol_id</t>
@@ -11015,7 +11549,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -11037,7 +11571,7 @@
       <c r="O5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -11055,10 +11589,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="6" min="1" style="3" width="25.6640625"/>
+    <col width="25.6640625" customWidth="1" style="3" min="1" max="6"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>RETAIL NAME</t>
@@ -11090,7 +11624,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="68" r="2" s="3">
+    <row r="2" ht="68" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>The retail name of the kit/reagent.</t>
@@ -11122,7 +11656,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="85" r="3" s="3">
+    <row r="3" ht="85" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> For example: SureCell WTA 3' Library Prep Kit; CytoTune iPS 2.0 Sendai Reprogramming Kit</t>
@@ -11154,7 +11688,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>ipsc_induction_protocol.reagents.retail_name</t>
@@ -11186,7 +11720,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -11199,7 +11733,7 @@
       <c r="F5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -11217,14 +11751,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="25.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="32.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="25.6640625"/>
-    <col customWidth="1" max="4" min="4" style="3" width="33.6640625"/>
-    <col customWidth="1" max="7" min="5" style="3" width="25.6640625"/>
+    <col width="25.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="32.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="25.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="33.6640625" customWidth="1" style="3" min="4" max="4"/>
+    <col width="25.6640625" customWidth="1" style="3" min="5" max="7"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>CHANNEL ID (Required)</t>
@@ -11261,7 +11795,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="85" r="2" s="3">
+    <row r="2" ht="85" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>User given ID.  If there is an accompanying codebook, this name should correspond to the channel id used in the codebook.</t>
@@ -11298,7 +11832,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="51" r="3" s="3">
+    <row r="3" ht="51" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> For example: 1; A</t>
@@ -11335,7 +11869,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>imaging_protocol.channel.channel_id</t>
@@ -11372,7 +11906,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -11386,7 +11920,7 @@
       <c r="G5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -11404,21 +11938,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="5" min="1" style="3" width="25.6640625"/>
-    <col customWidth="1" max="6" min="6" style="3" width="28.6640625"/>
-    <col hidden="1" max="8" min="7" style="3"/>
-    <col customWidth="1" max="9" min="9" style="3" width="41.6640625"/>
-    <col customWidth="1" max="10" min="10" style="3" width="44.6640625"/>
-    <col customWidth="1" max="11" min="11" style="3" width="42.6640625"/>
-    <col customWidth="1" max="12" min="12" style="3" width="46.6640625"/>
-    <col customWidth="1" max="13" min="13" style="3" width="41.6640625"/>
-    <col customWidth="1" max="14" min="14" style="3" width="35.6640625"/>
-    <col customWidth="1" max="15" min="15" style="3" width="25.6640625"/>
-    <col hidden="1" max="17" min="16" style="3"/>
-    <col customWidth="1" max="18" min="18" style="3" width="25.6640625"/>
+    <col width="25.6640625" customWidth="1" style="3" min="1" max="5"/>
+    <col width="28.6640625" customWidth="1" style="3" min="6" max="6"/>
+    <col hidden="1" style="3" min="7" max="8"/>
+    <col width="41.6640625" customWidth="1" style="3" min="9" max="9"/>
+    <col width="44.6640625" customWidth="1" style="3" min="10" max="10"/>
+    <col width="42.6640625" customWidth="1" style="3" min="11" max="11"/>
+    <col width="46.6640625" customWidth="1" style="3" min="12" max="12"/>
+    <col width="41.6640625" customWidth="1" style="3" min="13" max="13"/>
+    <col width="35.6640625" customWidth="1" style="3" min="14" max="14"/>
+    <col width="25.6640625" customWidth="1" style="3" min="15" max="15"/>
+    <col hidden="1" style="3" min="16" max="17"/>
+    <col width="25.6640625" customWidth="1" style="3" min="18" max="18"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>PROBE LABEL (Required)</t>
@@ -11510,7 +12044,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>The label of a probe used to detect target in this experiment.</t>
@@ -11602,7 +12136,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="153" r="3" s="3">
+    <row r="3" ht="153" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> For example: ACTA1; cFos</t>
@@ -11694,7 +12228,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>imaging_protocol.probe.probe_label</t>
@@ -11786,7 +12320,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -11811,7 +12345,7 @@
       <c r="R5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -11829,10 +12363,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="3" min="1" style="3" width="25.6640625"/>
+    <col width="25.6640625" customWidth="1" style="3" min="1" max="3"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>PARENT</t>
@@ -11849,7 +12383,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="2" s="3">
+    <row r="2" ht="17" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>The individual's parent.</t>
@@ -11866,7 +12400,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="34" r="3" s="3">
+    <row r="3" ht="34" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Enter the ID of the parent of this individual.</t>
@@ -11883,7 +12417,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>donor_organism.familial_relationships.parent</t>
@@ -11900,7 +12434,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -11910,7 +12444,7 @@
       <c r="C5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -11928,13 +12462,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="25.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="28.6640625"/>
-    <col customWidth="1" max="5" min="3" style="3" width="25.6640625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="3" width="24"/>
+    <col width="25.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="28.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="25.6640625" customWidth="1" style="3" min="3" max="5"/>
+    <col width="24" bestFit="1" customWidth="1" style="3" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>AUTHORS (Required)</t>
@@ -11966,7 +12500,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="113" r="2" s="3">
+    <row r="2" ht="113" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A list of authors associated with the publication.</t>
@@ -11998,7 +12532,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="68" r="3" s="3">
+    <row r="3" ht="68" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>List each author in 'surname initials' format. For example: Doe JD</t>
@@ -12062,7 +12596,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -12075,14 +12609,30 @@
       <c r="F5" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Reyfman PA||Walter JM||Joshi N||Anekalla KR||McQuattie-Pimentel AC||Chiu S||Fernandez R||Akbarpour M||Chen CI||Ren Z||Verma R||Abdala-Valencia H||Nam K||Chi M||Han S||Gonzalez-Gonzalez FJ||Soberanes S||Watanabe S||Williams KJN||Flozak AS||Nicholson TT||Morgan VK||Winter DR||Hinchcliff M||Hrusch CL||Guzy RD||Bonham CA||Sperling AI||Bag R||Hamanaka RB||Mutlu GM||Yeldandi AV||Marshall SA||Shilatifard A||Amaral LAN||Perlman H||Sznajder JI||Argento AC||Gillespie CT||Dematte J||Jain M||Singer BD||Ridge KM||Lam AP||Bharat A||Bhorade SM||Gottardi CJ||Budinger GRS||Misharin AV</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Single-Cell Transcriptomic Analysis of Human Lung Provides Insights into the Pathobiology of Pulmonary Fibrosis.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10.1164/rccm.201712-2410OC</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>30554520</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -12318,7 +12868,7 @@
     <hyperlink ref="A26" r:id="rId25"/>
     <hyperlink ref="A27" r:id="rId26"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -12328,7 +12878,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -12336,11 +12886,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="2" min="1" style="3" width="25.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="31.6640625"/>
+    <col width="25.6640625" customWidth="1" style="3" min="1" max="2"/>
+    <col width="31.6640625" customWidth="1" style="3" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>GRANT TITLE</t>
@@ -12357,7 +12907,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="34" r="2" s="3">
+    <row r="2" ht="34" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>The name of the grant funding the project.</t>
@@ -12374,7 +12924,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="68" r="3" s="3">
+    <row r="3" ht="68" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Enter a title of approximately 30 words. For example: Study of single cells in the human body.</t>
@@ -12391,7 +12941,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>project.funders.grant_title</t>
@@ -12408,7 +12958,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -12417,9 +12967,224 @@
       <c r="B5" s="1" t="n"/>
       <c r="C5" s="1" t="n"/>
     </row>
-    <row r="6"/>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>I01 CX001777</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CSRD VA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>K08 HL125940</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NHLBI NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>L30 HL134087</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NHLBI NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>K01 AR066579</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NIAMS NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>UL1 TR001863</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NCATS NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>K08 HL128867</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NHLBI NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>P01 HL071643</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NHLBI NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>U19 AI135964</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NIAID NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>UL1 TR001422</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NCATS NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>R21 AI126031</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NIAID NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>R01 ES015024</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NIEHS NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>R01 HL128194</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NHLBI NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>R01 HL134375</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NHLBI NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>R56 HL135124</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>NHLBI NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>R01 HL134800</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NHLBI NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>T32 HL076139</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NHLBI NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>K23 HL143135</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NHLBI NIH HHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>P01 AG049665</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>NIA NIH HHS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -12437,45 +13202,45 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="28.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="25.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="26.6640625"/>
-    <col customWidth="1" max="11" min="4" style="3" width="25.6640625"/>
-    <col hidden="1" max="13" min="12" style="3"/>
-    <col customWidth="1" max="14" min="14" style="3" width="25.6640625"/>
-    <col hidden="1" max="16" min="15" style="3"/>
-    <col customWidth="1" max="17" min="17" style="3" width="25.6640625"/>
-    <col hidden="1" max="19" min="18" style="3"/>
-    <col customWidth="1" max="20" min="20" style="3" width="25.6640625"/>
-    <col customWidth="1" max="21" min="21" style="3" width="30.6640625"/>
-    <col customWidth="1" max="23" min="22" style="3" width="25.6640625"/>
-    <col hidden="1" max="25" min="24" style="3"/>
-    <col customWidth="1" max="26" min="26" style="3" width="28.6640625"/>
-    <col hidden="1" max="28" min="27" style="3"/>
-    <col customWidth="1" max="29" min="29" style="3" width="25.6640625"/>
-    <col customWidth="1" hidden="1" max="31" min="30" style="3" width="8.83203125"/>
-    <col customWidth="1" max="33" min="32" style="3" width="25.6640625"/>
-    <col customWidth="1" max="34" min="34" style="3" width="28.6640625"/>
-    <col customWidth="1" max="37" min="35" style="3" width="25.6640625"/>
-    <col customWidth="1" max="38" min="38" style="3" width="31.6640625"/>
-    <col customWidth="1" max="46" min="39" style="3" width="25.6640625"/>
-    <col hidden="1" max="48" min="47" style="3"/>
-    <col customWidth="1" max="50" min="49" style="3" width="25.6640625"/>
-    <col hidden="1" max="52" min="51" style="3"/>
-    <col customWidth="1" max="54" min="53" style="3" width="25.6640625"/>
-    <col hidden="1" max="56" min="55" style="3"/>
-    <col customWidth="1" max="57" min="57" style="3" width="27.6640625"/>
-    <col customWidth="1" max="58" min="58" style="3" width="26.6640625"/>
-    <col hidden="1" max="60" min="59" style="3"/>
-    <col customWidth="1" max="70" min="61" style="3" width="25.6640625"/>
-    <col hidden="1" max="72" min="71" style="3"/>
-    <col customWidth="1" max="73" min="73" style="3" width="25.6640625"/>
-    <col hidden="1" max="75" min="74" style="3"/>
-    <col customWidth="1" max="76" min="76" style="3" width="25.6640625"/>
-    <col customWidth="1" max="77" min="77" style="3" width="37.6640625"/>
+    <col width="28.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="25.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="26.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="11"/>
+    <col hidden="1" style="3" min="12" max="13"/>
+    <col width="25.6640625" customWidth="1" style="3" min="14" max="14"/>
+    <col hidden="1" style="3" min="15" max="16"/>
+    <col width="25.6640625" customWidth="1" style="3" min="17" max="17"/>
+    <col hidden="1" style="3" min="18" max="19"/>
+    <col width="25.6640625" customWidth="1" style="3" min="20" max="20"/>
+    <col width="30.6640625" customWidth="1" style="3" min="21" max="21"/>
+    <col width="25.6640625" customWidth="1" style="3" min="22" max="23"/>
+    <col hidden="1" style="3" min="24" max="25"/>
+    <col width="28.6640625" customWidth="1" style="3" min="26" max="26"/>
+    <col hidden="1" style="3" min="27" max="28"/>
+    <col width="25.6640625" customWidth="1" style="3" min="29" max="29"/>
+    <col hidden="1" width="8.83203125" customWidth="1" style="3" min="30" max="31"/>
+    <col width="25.6640625" customWidth="1" style="3" min="32" max="33"/>
+    <col width="28.6640625" customWidth="1" style="3" min="34" max="34"/>
+    <col width="25.6640625" customWidth="1" style="3" min="35" max="37"/>
+    <col width="31.6640625" customWidth="1" style="3" min="38" max="38"/>
+    <col width="25.6640625" customWidth="1" style="3" min="39" max="46"/>
+    <col hidden="1" style="3" min="47" max="48"/>
+    <col width="25.6640625" customWidth="1" style="3" min="49" max="50"/>
+    <col hidden="1" style="3" min="51" max="52"/>
+    <col width="25.6640625" customWidth="1" style="3" min="53" max="54"/>
+    <col hidden="1" style="3" min="55" max="56"/>
+    <col width="27.6640625" customWidth="1" style="3" min="57" max="57"/>
+    <col width="26.6640625" customWidth="1" style="3" min="58" max="58"/>
+    <col hidden="1" style="3" min="59" max="60"/>
+    <col width="25.6640625" customWidth="1" style="3" min="61" max="70"/>
+    <col hidden="1" style="3" min="71" max="72"/>
+    <col width="25.6640625" customWidth="1" style="3" min="73" max="73"/>
+    <col hidden="1" style="3" min="74" max="75"/>
+    <col width="25.6640625" customWidth="1" style="3" min="76" max="76"/>
+    <col width="37.6640625" customWidth="1" style="3" min="77" max="77"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>DONOR ORGANISM ID (Required)</t>
@@ -12862,7 +13627,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the biomaterial.</t>
@@ -13249,7 +14014,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="153" r="3" s="3">
+    <row r="3" ht="153" customHeight="1" s="3">
       <c r="A3" s="2" t="n"/>
       <c r="B3" s="2" t="n"/>
       <c r="C3" s="2" t="n"/>
@@ -13612,7 +14377,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>donor_organism.biomaterial_core.biomaterial_id</t>
@@ -13999,7 +14764,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -14083,7 +14848,7 @@
       <c r="BY5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -14101,37 +14866,37 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="36.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="27.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="34.6640625"/>
-    <col customWidth="1" max="10" min="4" style="3" width="25.6640625"/>
-    <col hidden="1" max="12" min="11" style="3"/>
-    <col customWidth="1" max="13" min="13" style="3" width="25.6640625"/>
-    <col hidden="1" max="15" min="14" style="3"/>
-    <col customWidth="1" max="16" min="16" style="3" width="25.6640625"/>
-    <col hidden="1" max="18" min="17" style="3"/>
-    <col customWidth="1" max="19" min="19" style="3" width="25.6640625"/>
-    <col customWidth="1" hidden="1" max="21" min="20" style="3" width="8.83203125"/>
-    <col customWidth="1" max="32" min="22" style="3" width="25.6640625"/>
-    <col hidden="1" max="34" min="33" style="3"/>
-    <col customWidth="1" max="36" min="35" style="3" width="25.6640625"/>
-    <col customWidth="1" max="37" min="37" style="3" width="32.6640625"/>
-    <col customWidth="1" max="38" min="38" style="3" width="35.6640625"/>
-    <col customWidth="1" max="39" min="39" style="3" width="33.6640625"/>
-    <col customWidth="1" max="40" min="40" style="3" width="37.6640625"/>
-    <col customWidth="1" max="41" min="41" style="3" width="32.6640625"/>
-    <col customWidth="1" max="42" min="42" style="3" width="26.6640625"/>
-    <col customWidth="1" max="43" min="43" style="3" width="34.6640625"/>
-    <col customWidth="1" max="44" min="44" style="3" width="33.6640625"/>
-    <col customWidth="1" max="53" min="45" style="3" width="25.6640625"/>
-    <col hidden="1" max="55" min="54" style="3"/>
-    <col customWidth="1" max="56" min="56" style="3" width="25.6640625"/>
-    <col hidden="1" max="58" min="57" style="3"/>
-    <col customWidth="1" max="59" min="59" style="3" width="25.6640625"/>
-    <col customWidth="1" max="60" min="60" style="3" width="37.6640625"/>
+    <col width="36.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="27.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="34.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="10"/>
+    <col hidden="1" style="3" min="11" max="12"/>
+    <col width="25.6640625" customWidth="1" style="3" min="13" max="13"/>
+    <col hidden="1" style="3" min="14" max="15"/>
+    <col width="25.6640625" customWidth="1" style="3" min="16" max="16"/>
+    <col hidden="1" style="3" min="17" max="18"/>
+    <col width="25.6640625" customWidth="1" style="3" min="19" max="19"/>
+    <col hidden="1" width="8.83203125" customWidth="1" style="3" min="20" max="21"/>
+    <col width="25.6640625" customWidth="1" style="3" min="22" max="32"/>
+    <col hidden="1" style="3" min="33" max="34"/>
+    <col width="25.6640625" customWidth="1" style="3" min="35" max="36"/>
+    <col width="32.6640625" customWidth="1" style="3" min="37" max="37"/>
+    <col width="35.6640625" customWidth="1" style="3" min="38" max="38"/>
+    <col width="33.6640625" customWidth="1" style="3" min="39" max="39"/>
+    <col width="37.6640625" customWidth="1" style="3" min="40" max="40"/>
+    <col width="32.6640625" customWidth="1" style="3" min="41" max="41"/>
+    <col width="26.6640625" customWidth="1" style="3" min="42" max="42"/>
+    <col width="34.6640625" customWidth="1" style="3" min="43" max="43"/>
+    <col width="33.6640625" customWidth="1" style="3" min="44" max="44"/>
+    <col width="25.6640625" customWidth="1" style="3" min="45" max="53"/>
+    <col hidden="1" style="3" min="54" max="55"/>
+    <col width="25.6640625" customWidth="1" style="3" min="56" max="56"/>
+    <col hidden="1" style="3" min="57" max="58"/>
+    <col width="25.6640625" customWidth="1" style="3" min="59" max="59"/>
+    <col width="37.6640625" customWidth="1" style="3" min="60" max="60"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>SPECIMEN FROM ORGANISM ID (Required)</t>
@@ -14433,7 +15198,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the biomaterial.</t>
@@ -14735,7 +15500,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="153" r="3" s="3">
+    <row r="3" ht="153" customHeight="1" s="3">
       <c r="A3" s="2" t="n"/>
       <c r="B3" s="2" t="n"/>
       <c r="C3" s="2" t="n"/>
@@ -15009,7 +15774,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>specimen_from_organism.biomaterial_core.biomaterial_id</t>
@@ -15311,7 +16076,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -15470,7 +16235,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -15488,34 +16253,34 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="29.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="25.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="27.6640625"/>
-    <col customWidth="1" max="12" min="4" style="3" width="25.6640625"/>
-    <col hidden="1" max="14" min="13" style="3"/>
-    <col customWidth="1" max="22" min="15" style="3" width="25.6640625"/>
-    <col customWidth="1" max="23" min="23" style="3" width="26.6640625"/>
-    <col customWidth="1" max="26" min="24" style="3" width="25.6640625"/>
-    <col hidden="1" max="28" min="27" style="3"/>
-    <col customWidth="1" max="29" min="29" style="3" width="25.6640625"/>
-    <col hidden="1" max="31" min="30" style="3"/>
-    <col customWidth="1" max="35" min="32" style="3" width="25.6640625"/>
-    <col customWidth="1" max="36" min="36" style="3" width="27.6640625"/>
-    <col customWidth="1" max="37" min="37" style="3" width="26.6640625"/>
-    <col hidden="1" max="39" min="38" style="3"/>
-    <col customWidth="1" max="40" min="40" style="3" width="25.6640625"/>
-    <col customWidth="1" max="41" min="41" style="3" width="42.6640625"/>
-    <col customWidth="1" max="42" min="42" style="3" width="35.6640625"/>
-    <col customWidth="1" max="43" min="43" style="3" width="33.6640625"/>
-    <col customWidth="1" max="52" min="44" style="3" width="25.6640625"/>
-    <col hidden="1" max="54" min="53" style="3"/>
-    <col customWidth="1" max="55" min="55" style="3" width="25.6640625"/>
-    <col hidden="1" max="57" min="56" style="3"/>
-    <col customWidth="1" max="58" min="58" style="3" width="25.6640625"/>
-    <col customWidth="1" max="59" min="59" style="3" width="37.6640625"/>
+    <col width="29.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="25.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="27.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="12"/>
+    <col hidden="1" style="3" min="13" max="14"/>
+    <col width="25.6640625" customWidth="1" style="3" min="15" max="22"/>
+    <col width="26.6640625" customWidth="1" style="3" min="23" max="23"/>
+    <col width="25.6640625" customWidth="1" style="3" min="24" max="26"/>
+    <col hidden="1" style="3" min="27" max="28"/>
+    <col width="25.6640625" customWidth="1" style="3" min="29" max="29"/>
+    <col hidden="1" style="3" min="30" max="31"/>
+    <col width="25.6640625" customWidth="1" style="3" min="32" max="35"/>
+    <col width="27.6640625" customWidth="1" style="3" min="36" max="36"/>
+    <col width="26.6640625" customWidth="1" style="3" min="37" max="37"/>
+    <col hidden="1" style="3" min="38" max="39"/>
+    <col width="25.6640625" customWidth="1" style="3" min="40" max="40"/>
+    <col width="42.6640625" customWidth="1" style="3" min="41" max="41"/>
+    <col width="35.6640625" customWidth="1" style="3" min="42" max="42"/>
+    <col width="33.6640625" customWidth="1" style="3" min="43" max="43"/>
+    <col width="25.6640625" customWidth="1" style="3" min="44" max="52"/>
+    <col hidden="1" style="3" min="53" max="54"/>
+    <col width="25.6640625" customWidth="1" style="3" min="55" max="55"/>
+    <col hidden="1" style="3" min="56" max="57"/>
+    <col width="25.6640625" customWidth="1" style="3" min="58" max="58"/>
+    <col width="37.6640625" customWidth="1" style="3" min="59" max="59"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>CELL SUSPENSION ID (Required)</t>
@@ -15812,7 +16577,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the biomaterial.</t>
@@ -16109,7 +16874,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="170" r="3" s="3">
+    <row r="3" ht="170" customHeight="1" s="3">
       <c r="A3" s="2" t="n"/>
       <c r="B3" s="2" t="n"/>
       <c r="C3" s="2" t="n"/>
@@ -16378,7 +17143,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>cell_suspension.biomaterial_core.biomaterial_id</t>
@@ -16675,7 +17440,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -16801,7 +17566,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -16819,31 +17584,31 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="10" min="1" style="3" width="25.6640625"/>
-    <col hidden="1" max="12" min="11" style="3"/>
-    <col customWidth="1" max="13" min="13" style="3" width="25.6640625"/>
-    <col hidden="1" max="15" min="14" style="3"/>
-    <col customWidth="1" max="16" min="16" style="3" width="25.6640625"/>
-    <col hidden="1" max="18" min="17" style="3"/>
-    <col customWidth="1" max="20" min="19" style="3" width="25.6640625"/>
-    <col hidden="1" max="22" min="21" style="3"/>
-    <col customWidth="1" max="24" min="23" style="3" width="25.6640625"/>
-    <col hidden="1" max="26" min="25" style="3"/>
-    <col customWidth="1" max="29" min="27" style="3" width="25.6640625"/>
-    <col customWidth="1" max="30" min="30" style="3" width="26.6640625"/>
-    <col customWidth="1" max="31" min="31" style="3" width="25.6640625"/>
-    <col customWidth="1" max="32" min="32" style="3" width="42.6640625"/>
-    <col customWidth="1" max="33" min="33" style="3" width="43.6640625"/>
-    <col customWidth="1" max="34" min="34" style="3" width="38.6640625"/>
-    <col customWidth="1" max="43" min="35" style="3" width="25.6640625"/>
-    <col hidden="1" max="45" min="44" style="3"/>
-    <col customWidth="1" max="46" min="46" style="3" width="25.6640625"/>
-    <col hidden="1" max="48" min="47" style="3"/>
-    <col customWidth="1" max="49" min="49" style="3" width="25.6640625"/>
-    <col customWidth="1" max="50" min="50" style="3" width="37.6640625"/>
+    <col width="25.6640625" customWidth="1" style="3" min="1" max="10"/>
+    <col hidden="1" style="3" min="11" max="12"/>
+    <col width="25.6640625" customWidth="1" style="3" min="13" max="13"/>
+    <col hidden="1" style="3" min="14" max="15"/>
+    <col width="25.6640625" customWidth="1" style="3" min="16" max="16"/>
+    <col hidden="1" style="3" min="17" max="18"/>
+    <col width="25.6640625" customWidth="1" style="3" min="19" max="20"/>
+    <col hidden="1" style="3" min="21" max="22"/>
+    <col width="25.6640625" customWidth="1" style="3" min="23" max="24"/>
+    <col hidden="1" style="3" min="25" max="26"/>
+    <col width="25.6640625" customWidth="1" style="3" min="27" max="29"/>
+    <col width="26.6640625" customWidth="1" style="3" min="30" max="30"/>
+    <col width="25.6640625" customWidth="1" style="3" min="31" max="31"/>
+    <col width="42.6640625" customWidth="1" style="3" min="32" max="32"/>
+    <col width="43.6640625" customWidth="1" style="3" min="33" max="33"/>
+    <col width="38.6640625" customWidth="1" style="3" min="34" max="34"/>
+    <col width="25.6640625" customWidth="1" style="3" min="35" max="43"/>
+    <col hidden="1" style="3" min="44" max="45"/>
+    <col width="25.6640625" customWidth="1" style="3" min="46" max="46"/>
+    <col hidden="1" style="3" min="47" max="48"/>
+    <col width="25.6640625" customWidth="1" style="3" min="49" max="49"/>
+    <col width="37.6640625" customWidth="1" style="3" min="50" max="50"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>ORGANOID ID (Required)</t>
@@ -17095,7 +17860,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the biomaterial.</t>
@@ -17347,7 +18112,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="136" r="3" s="3">
+    <row r="3" ht="136" customHeight="1" s="3">
       <c r="A3" s="2" t="n"/>
       <c r="B3" s="2" t="n"/>
       <c r="C3" s="2" t="n"/>
@@ -17571,7 +18336,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>organoid.biomaterial_core.biomaterial_id</t>
@@ -17823,7 +18588,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -17880,7 +18645,7 @@
       <c r="AX5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -17898,23 +18663,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="29.6640625"/>
-    <col customWidth="1" max="2" min="2" style="3" width="25.6640625"/>
-    <col customWidth="1" max="3" min="3" style="3" width="27.6640625"/>
-    <col customWidth="1" max="10" min="4" style="3" width="25.6640625"/>
-    <col customWidth="1" max="11" min="11" style="3" width="33.6640625"/>
-    <col customWidth="1" max="12" min="12" style="3" width="26.6640625"/>
-    <col hidden="1" max="14" min="13" style="3"/>
-    <col customWidth="1" max="16" min="15" style="3" width="42.6640625"/>
-    <col customWidth="1" max="25" min="17" style="3" width="25.6640625"/>
-    <col hidden="1" max="27" min="26" style="3"/>
-    <col customWidth="1" max="28" min="28" style="3" width="25.6640625"/>
-    <col hidden="1" max="30" min="29" style="3"/>
-    <col customWidth="1" max="31" min="31" style="3" width="25.6640625"/>
-    <col customWidth="1" max="32" min="32" style="3" width="37.6640625"/>
+    <col width="29.6640625" customWidth="1" style="3" min="1" max="1"/>
+    <col width="25.6640625" customWidth="1" style="3" min="2" max="2"/>
+    <col width="27.6640625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="25.6640625" customWidth="1" style="3" min="4" max="10"/>
+    <col width="33.6640625" customWidth="1" style="3" min="11" max="11"/>
+    <col width="26.6640625" customWidth="1" style="3" min="12" max="12"/>
+    <col hidden="1" style="3" min="13" max="14"/>
+    <col width="42.6640625" customWidth="1" style="3" min="15" max="16"/>
+    <col width="25.6640625" customWidth="1" style="3" min="17" max="25"/>
+    <col hidden="1" style="3" min="26" max="27"/>
+    <col width="25.6640625" customWidth="1" style="3" min="28" max="28"/>
+    <col hidden="1" style="3" min="29" max="30"/>
+    <col width="25.6640625" customWidth="1" style="3" min="31" max="31"/>
+    <col width="37.6640625" customWidth="1" style="3" min="32" max="32"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="30" r="1" s="3">
+    <row r="1" ht="30" customHeight="1" s="3">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>IMAGED SPECIMEN ID (Required)</t>
@@ -18076,7 +18841,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="306" r="2" s="3">
+    <row r="2" ht="306" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>A unique ID for the biomaterial.</t>
@@ -18238,7 +19003,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="136" r="3" s="3">
+    <row r="3" ht="136" customHeight="1" s="3">
       <c r="A3" s="2" t="n"/>
       <c r="B3" s="2" t="n"/>
       <c r="C3" s="2" t="n"/>
@@ -18372,7 +19137,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="3">
+    <row r="4" hidden="1" s="3">
       <c r="A4" t="inlineStr">
         <is>
           <t>imaged_specimen.biomaterial_core.biomaterial_id</t>
@@ -18534,7 +19299,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5" s="3">
+    <row r="5" ht="30" customHeight="1" s="3">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FILL OUT INFORMATION BELOW THIS ROW</t>
@@ -18573,6 +19338,6 @@
       <c r="AF5" s="1" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>